<commit_message>
set for phones 2 reprocess
</commit_message>
<xml_diff>
--- a/tablets_matches.xlsx
+++ b/tablets_matches.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -401,12 +401,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">acer aspire 1  </t>
+          <t xml:space="preserve">iphone xr blanco  </t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>acer aspire 5 a515-55 - ordenador portátil 15.6" fullhd (intel core i5-1035g1, 8gb ram, 256gb ssd, uma graphics, windows 10 home), color plata - teclado qwerty español</t>
+          <t>apple iphone xr (128 gb) - en blanco</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -416,19 +416,19 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>https://www.amazon.es/Acer-Aspire-Port%C3%A1til-i5-1035G1-Graphics/dp/B08F5JK7VR/ref=sr_1_5?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-5</t>
+          <t>https://www.amazon.es/Apple-iPhone-XR-128-GB-Blanco/dp/B08L71BVYB/ref=ice_ac_b_dpb?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+xr+blanco&amp;qid=1631026080&amp;s=electronics&amp;sr=1-3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">acer aspire 1  </t>
+          <t xml:space="preserve">iphone xr blanco  </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>acer aspire 5 a515-44 - ordenador portátil 15.6" full hd, laptop (amd ryzen 7 4700u, 8 gb ram, 512 gb ssd, uma graphics, comfyview, endless os), pc portátil color negro - teclado qwerty español</t>
+          <t>apple iphone xr 64 gb blanco (reacondicionado)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -438,19 +438,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.amazon.es/Acer-Aspire-A515-44-Ordenador-ComfyView/dp/B08WX5F7LM/ref=sr_1_7?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-7</t>
+          <t>https://www.amazon.es/Apple-iPhone-XR-Blanco-Reacondicionado/dp/B07N9N4VZ9/ref=sr_1_4?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+xr+blanco&amp;qid=1631026080&amp;s=electronics&amp;sr=1-4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">acer aspire 1  </t>
+          <t xml:space="preserve">iphone xr blanco  </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>acer aspire 5 a515-56g - ordenador portátil 15.6" full hd, laptop (intel core i7-1165g7, 8 gb ram, 512 gb ssd, nvidia geforce mx350 2gb, comfyview, sin os), pc portátil plata, teclado qwerty español</t>
+          <t>apple iphone xr (64 gb) - en blanco</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -460,19 +460,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.amazon.es/Acer-Aspire-A515-56G-Ordenador-i7-1165G7/dp/B08PX44Q8J/ref=sr_1_11?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-11</t>
+          <t>https://www.amazon.es/Apple-iPhone-XR-64-GB-Blanco/dp/B08L6ZJPTK/ref=sr_1_5?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+xr+blanco&amp;qid=1631026080&amp;s=electronics&amp;sr=1-5</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">acer aspire 1  </t>
+          <t xml:space="preserve">iphone xr blanco  </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>acer aspire 5 a515-56 - ordenador portátil 15.6" full hd, laptop (intel core i7-1165g7, 8 gb ram, 512 gb ssd, intel iris xe graphics, comfyview, sin os), pc portátil plata, teclado qwerty español</t>
+          <t>apple iphone xr 128 gb blanco (reacondicionado)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -482,56 +482,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.amazon.es/Acer-Aspire-A515-56-Ordenador-i7-1165G7/dp/B08PX3C2SW/ref=sr_1_15?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-15</t>
+          <t>https://www.amazon.es/Apple-iPhone-128-Blanco-Reacondicionado/dp/B07N9HM41P/ref=sr_1_6?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=iphone+xr+blanco&amp;qid=1631026080&amp;s=electronics&amp;sr=1-6</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">acer aspire 1  </t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>acer aspire 5 a515-55 - ordenador portátil 15.6" full hd, laptop (intel core i5-1035g1, 16gb ram, 512gb ssd, uma graphics, windows 10 home), pc portátil color plata - teclado qwerty español</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://www.amazon.es/Acer-Aspire-Port%C3%A1til-i5-1035G1-Graphics/dp/B08F5KDS6M/ref=sr_1_28?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-28</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">acer aspire 1  </t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>acer aspire 3 a315-56-35rx 15.6" i3-1005g1 1.2ghz ram 8gb 256gb ssd windows 10 home black nx.hs5et.001</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://www.amazon.es/ASPIRE-A315-56-35RX-I3-1005G1-WINDOWS-NX-HS5ET-001/dp/B094X7PTQV/ref=sr_1_29?__mk_es_ES=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=acer+aspire+1&amp;qid=1631022114&amp;s=electronics&amp;sr=1-29</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
         <is>
           <t>############################################################################</t>
         </is>

</xml_diff>